<commit_message>
added all cucumber bdd tests for a2
</commit_message>
<xml_diff>
--- a/MaxwellMichael-grid-a2.xlsx
+++ b/MaxwellMichael-grid-a2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PROLE\Documents\GitHub\poker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PROLE\eclipse-workspace\cucumber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C975E42-0274-42C4-B920-712BA20EB4FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560896C0-FF22-480F-A9AC-8FF82FE41305}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="169">
   <si>
     <t>First Name</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>maximum</t>
-  </si>
-  <si>
-    <t>yes/no</t>
   </si>
   <si>
     <t xml:space="preserve">two pairs with the same highest pair for each participant, </t>
@@ -514,6 +511,48 @@
   </si>
   <si>
     <t>Maxwell</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>hand_beats.feature</t>
+  </si>
+  <si>
+    <t>detect_hand.feature</t>
+  </si>
+  <si>
+    <t>11, 18</t>
+  </si>
+  <si>
+    <t>19, 25</t>
+  </si>
+  <si>
+    <t>26, 31</t>
+  </si>
+  <si>
+    <t>32, 37</t>
+  </si>
+  <si>
+    <t>38, 43</t>
+  </si>
+  <si>
+    <t>44, 49</t>
+  </si>
+  <si>
+    <t>50, 55</t>
+  </si>
+  <si>
+    <t>56, 61</t>
+  </si>
+  <si>
+    <t>62, 67</t>
+  </si>
+  <si>
+    <t>card_exchange.feature</t>
+  </si>
+  <si>
+    <t>same_hand.feature</t>
   </si>
 </sst>
 </file>
@@ -2056,7 +2095,7 @@
   <dimension ref="A1:IV152"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2071,16 +2110,16 @@
   <sheetData>
     <row r="1" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
@@ -2094,16 +2133,16 @@
     </row>
     <row r="2" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -2124,7 +2163,7 @@
         <v>101006277</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -2153,10 +2192,10 @@
     </row>
     <row r="5" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>150</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="12"/>
@@ -2173,7 +2212,7 @@
     <row r="6" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>3</v>
@@ -2182,7 +2221,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -2196,10 +2235,10 @@
     </row>
     <row r="7" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="12"/>
@@ -2216,17 +2255,21 @@
     </row>
     <row r="8" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="12">
         <v>3</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>157</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -2238,16 +2281,18 @@
     </row>
     <row r="9" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="12">
         <v>2</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="F9" s="29"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -2260,16 +2305,18 @@
     </row>
     <row r="10" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="12">
         <v>2</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="29" t="s">
+        <v>160</v>
+      </c>
       <c r="F10" s="29"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -2282,16 +2329,18 @@
     </row>
     <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="12">
         <v>2</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="29" t="s">
+        <v>161</v>
+      </c>
       <c r="F11" s="29"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -2304,16 +2353,18 @@
     </row>
     <row r="12" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="12">
         <v>2</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="29" t="s">
+        <v>162</v>
+      </c>
       <c r="F12" s="29"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -2326,16 +2377,18 @@
     </row>
     <row r="13" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="12">
         <v>2</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="29" t="s">
+        <v>163</v>
+      </c>
       <c r="F13" s="29"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -2348,16 +2401,18 @@
     </row>
     <row r="14" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="12">
         <v>3</v>
       </c>
-      <c r="E14" s="29"/>
+      <c r="E14" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F14" s="29"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -2370,16 +2425,18 @@
     </row>
     <row r="15" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="12">
         <v>2</v>
       </c>
-      <c r="E15" s="29"/>
+      <c r="E15" s="29" t="s">
+        <v>165</v>
+      </c>
       <c r="F15" s="29"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -2396,16 +2453,18 @@
     </row>
     <row r="16" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="12">
         <v>2</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="29" t="s">
+        <v>166</v>
+      </c>
       <c r="F16" s="29"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -2442,7 +2501,7 @@
     </row>
     <row r="18" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="7"/>
@@ -2464,17 +2523,21 @@
     </row>
     <row r="19" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="12">
         <v>0.5</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
+      <c r="E19" s="29">
+        <v>11</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>156</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="20"/>
@@ -2490,16 +2553,18 @@
     </row>
     <row r="20" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="12">
         <v>0.5</v>
       </c>
-      <c r="E20" s="29"/>
+      <c r="E20" s="29">
+        <v>12</v>
+      </c>
       <c r="F20" s="29"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
@@ -2516,16 +2581,18 @@
     </row>
     <row r="21" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="12">
         <v>0.5</v>
       </c>
-      <c r="E21" s="29"/>
+      <c r="E21" s="29">
+        <v>13</v>
+      </c>
       <c r="F21" s="29"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -2539,16 +2606,18 @@
     </row>
     <row r="22" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="12">
         <v>0.5</v>
       </c>
-      <c r="E22" s="29"/>
+      <c r="E22" s="29">
+        <v>14</v>
+      </c>
       <c r="F22" s="29"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -2562,16 +2631,18 @@
     </row>
     <row r="23" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="12">
         <v>0.5</v>
       </c>
-      <c r="E23" s="29"/>
+      <c r="E23" s="29">
+        <v>15</v>
+      </c>
       <c r="F23" s="29"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -2585,16 +2656,18 @@
     </row>
     <row r="24" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="12">
         <v>0.5</v>
       </c>
-      <c r="E24" s="29"/>
+      <c r="E24" s="29">
+        <v>16</v>
+      </c>
       <c r="F24" s="29"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -2608,16 +2681,18 @@
     </row>
     <row r="25" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="12">
         <v>0.5</v>
       </c>
-      <c r="E25" s="29"/>
+      <c r="E25" s="29">
+        <v>17</v>
+      </c>
       <c r="F25" s="29"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -2631,16 +2706,18 @@
     </row>
     <row r="26" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="12">
         <v>0.5</v>
       </c>
-      <c r="E26" s="29"/>
+      <c r="E26" s="29">
+        <v>18</v>
+      </c>
       <c r="F26" s="29"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
@@ -2654,16 +2731,18 @@
     </row>
     <row r="27" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="12">
         <v>0.5</v>
       </c>
-      <c r="E27" s="29"/>
+      <c r="E27" s="29">
+        <v>19</v>
+      </c>
       <c r="F27" s="29"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -2677,16 +2756,18 @@
     </row>
     <row r="28" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="12">
         <v>0.5</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="29">
+        <v>21</v>
+      </c>
       <c r="F28" s="29"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -2700,16 +2781,18 @@
     </row>
     <row r="29" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="12">
         <v>0.5</v>
       </c>
-      <c r="E29" s="29"/>
+      <c r="E29" s="29">
+        <v>22</v>
+      </c>
       <c r="F29" s="29"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -2723,16 +2806,18 @@
     </row>
     <row r="30" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="12">
         <v>0.5</v>
       </c>
-      <c r="E30" s="29"/>
+      <c r="E30" s="29">
+        <v>23</v>
+      </c>
       <c r="F30" s="29"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -2746,16 +2831,18 @@
     </row>
     <row r="31" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="12">
         <v>0.5</v>
       </c>
-      <c r="E31" s="29"/>
+      <c r="E31" s="29">
+        <v>24</v>
+      </c>
       <c r="F31" s="29"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
@@ -2768,16 +2855,18 @@
     </row>
     <row r="32" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="12">
         <v>0.5</v>
       </c>
-      <c r="E32" s="29"/>
+      <c r="E32" s="29">
+        <v>25</v>
+      </c>
       <c r="F32" s="29"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
@@ -2791,16 +2880,18 @@
     </row>
     <row r="33" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="12">
         <v>0.5</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="29">
+        <v>26</v>
+      </c>
       <c r="F33" s="29"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
@@ -2814,16 +2905,18 @@
     </row>
     <row r="34" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C34" s="23"/>
       <c r="D34" s="12">
         <v>0.5</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="29">
+        <v>27</v>
+      </c>
       <c r="F34" s="29"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -2837,16 +2930,18 @@
     </row>
     <row r="35" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="12">
         <v>0.5</v>
       </c>
-      <c r="E35" s="29"/>
+      <c r="E35" s="29">
+        <v>28</v>
+      </c>
       <c r="F35" s="29"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
@@ -2860,16 +2955,18 @@
     </row>
     <row r="36" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="12">
         <v>0.5</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="E36" s="29">
+        <v>31</v>
+      </c>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
@@ -2883,16 +2980,18 @@
     </row>
     <row r="37" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="12">
         <v>0.5</v>
       </c>
-      <c r="E37" s="29"/>
+      <c r="E37" s="29">
+        <v>32</v>
+      </c>
       <c r="F37" s="29"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
@@ -2906,16 +3005,18 @@
     </row>
     <row r="38" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="12">
         <v>0.5</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="29">
+        <v>33</v>
+      </c>
       <c r="F38" s="29"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -2929,16 +3030,18 @@
     </row>
     <row r="39" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="12">
         <v>0.5</v>
       </c>
-      <c r="E39" s="29"/>
+      <c r="E39" s="29">
+        <v>34</v>
+      </c>
       <c r="F39" s="29"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -2952,16 +3055,18 @@
     </row>
     <row r="40" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C40" s="23"/>
       <c r="D40" s="12">
         <v>0.5</v>
       </c>
-      <c r="E40" s="29"/>
+      <c r="E40" s="29">
+        <v>35</v>
+      </c>
       <c r="F40" s="29"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
@@ -2975,16 +3080,18 @@
     </row>
     <row r="41" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="12">
         <v>0.5</v>
       </c>
-      <c r="E41" s="29"/>
+      <c r="E41" s="29">
+        <v>36</v>
+      </c>
       <c r="F41" s="29"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -2998,16 +3105,18 @@
     </row>
     <row r="42" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C42" s="23"/>
       <c r="D42" s="12">
         <v>0.5</v>
       </c>
-      <c r="E42" s="29"/>
+      <c r="E42" s="29">
+        <v>37</v>
+      </c>
       <c r="F42" s="29"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
@@ -3020,16 +3129,18 @@
     </row>
     <row r="43" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="12">
         <v>0.5</v>
       </c>
-      <c r="E43" s="29"/>
+      <c r="E43" s="29">
+        <v>41</v>
+      </c>
       <c r="F43" s="29"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -3042,16 +3153,18 @@
     </row>
     <row r="44" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="12">
         <v>0.5</v>
       </c>
-      <c r="E44" s="29"/>
+      <c r="E44" s="29">
+        <v>42</v>
+      </c>
       <c r="F44" s="29"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
@@ -3064,16 +3177,18 @@
     </row>
     <row r="45" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="12">
         <v>0.5</v>
       </c>
-      <c r="E45" s="29"/>
+      <c r="E45" s="29">
+        <v>43</v>
+      </c>
       <c r="F45" s="29"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
@@ -3086,16 +3201,18 @@
     </row>
     <row r="46" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="12">
         <v>0.5</v>
       </c>
-      <c r="E46" s="29"/>
+      <c r="E46" s="29">
+        <v>44</v>
+      </c>
       <c r="F46" s="29"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
@@ -3108,16 +3225,18 @@
     </row>
     <row r="47" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="12">
         <v>0.5</v>
       </c>
-      <c r="E47" s="29"/>
+      <c r="E47" s="29">
+        <v>45</v>
+      </c>
       <c r="F47" s="29"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
@@ -3130,16 +3249,18 @@
     </row>
     <row r="48" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="12">
         <v>0.5</v>
       </c>
-      <c r="E48" s="29"/>
+      <c r="E48" s="29">
+        <v>46</v>
+      </c>
       <c r="F48" s="29"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
@@ -3152,16 +3273,18 @@
     </row>
     <row r="49" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49" s="12">
         <v>0.5</v>
       </c>
-      <c r="E49" s="29"/>
+      <c r="E49" s="29">
+        <v>51</v>
+      </c>
       <c r="F49" s="29"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
@@ -3174,16 +3297,18 @@
     </row>
     <row r="50" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="12">
         <v>0.5</v>
       </c>
-      <c r="E50" s="29"/>
+      <c r="E50" s="29">
+        <v>52</v>
+      </c>
       <c r="F50" s="29"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
@@ -3196,16 +3321,18 @@
     </row>
     <row r="51" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51" s="12">
         <v>0.5</v>
       </c>
-      <c r="E51" s="29"/>
+      <c r="E51" s="29">
+        <v>53</v>
+      </c>
       <c r="F51" s="29"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -3218,16 +3345,18 @@
     </row>
     <row r="52" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C52" s="23"/>
       <c r="D52" s="12">
         <v>0.5</v>
       </c>
-      <c r="E52" s="29"/>
+      <c r="E52" s="29">
+        <v>54</v>
+      </c>
       <c r="F52" s="29"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
@@ -3240,16 +3369,18 @@
     </row>
     <row r="53" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C53" s="23"/>
       <c r="D53" s="12">
         <v>0.5</v>
       </c>
-      <c r="E53" s="29"/>
+      <c r="E53" s="29">
+        <v>55</v>
+      </c>
       <c r="F53" s="29"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
@@ -3262,16 +3393,18 @@
     </row>
     <row r="54" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C54" s="23"/>
       <c r="D54" s="12">
         <v>0.5</v>
       </c>
-      <c r="E54" s="29"/>
+      <c r="E54" s="29">
+        <v>61</v>
+      </c>
       <c r="F54" s="29"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -3284,16 +3417,18 @@
     </row>
     <row r="55" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C55" s="23"/>
       <c r="D55" s="12">
         <v>0.5</v>
       </c>
-      <c r="E55" s="29"/>
+      <c r="E55" s="29">
+        <v>62</v>
+      </c>
       <c r="F55" s="29"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
@@ -3306,16 +3441,18 @@
     </row>
     <row r="56" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C56" s="23"/>
       <c r="D56" s="12">
         <v>0.5</v>
       </c>
-      <c r="E56" s="29"/>
+      <c r="E56" s="29">
+        <v>63</v>
+      </c>
       <c r="F56" s="29"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
@@ -3328,16 +3465,18 @@
     </row>
     <row r="57" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C57" s="23"/>
       <c r="D57" s="12">
         <v>0.5</v>
       </c>
-      <c r="E57" s="29"/>
+      <c r="E57" s="29">
+        <v>64</v>
+      </c>
       <c r="F57" s="29"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
@@ -3350,16 +3489,18 @@
     </row>
     <row r="58" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C58" s="23"/>
       <c r="D58" s="12">
         <v>0.5</v>
       </c>
-      <c r="E58" s="29"/>
+      <c r="E58" s="29">
+        <v>71</v>
+      </c>
       <c r="F58" s="29"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
@@ -3372,16 +3513,18 @@
     </row>
     <row r="59" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C59" s="23"/>
       <c r="D59" s="12">
         <v>0.5</v>
       </c>
-      <c r="E59" s="29"/>
+      <c r="E59" s="29">
+        <v>72</v>
+      </c>
       <c r="F59" s="29"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
@@ -3394,16 +3537,18 @@
     </row>
     <row r="60" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C60" s="23"/>
       <c r="D60" s="12">
         <v>0.5</v>
       </c>
-      <c r="E60" s="29"/>
+      <c r="E60" s="29">
+        <v>73</v>
+      </c>
       <c r="F60" s="29"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
@@ -3416,16 +3561,18 @@
     </row>
     <row r="61" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C61" s="23"/>
       <c r="D61" s="12">
         <v>0.5</v>
       </c>
-      <c r="E61" s="29"/>
+      <c r="E61" s="29">
+        <v>81</v>
+      </c>
       <c r="F61" s="29"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
@@ -3438,16 +3585,18 @@
     </row>
     <row r="62" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="12">
         <v>0.5</v>
       </c>
-      <c r="E62" s="29"/>
+      <c r="E62" s="29">
+        <v>82</v>
+      </c>
       <c r="F62" s="29"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
@@ -3460,16 +3609,18 @@
     </row>
     <row r="63" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C63" s="23"/>
       <c r="D63" s="12">
         <v>0.5</v>
       </c>
-      <c r="E63" s="29"/>
+      <c r="E63" s="29">
+        <v>91</v>
+      </c>
       <c r="F63" s="29"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
@@ -3498,17 +3649,21 @@
     </row>
     <row r="65" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C65" s="23"/>
       <c r="D65" s="12">
         <v>0.5</v>
       </c>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
+      <c r="E65" s="29">
+        <v>20</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>156</v>
+      </c>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
@@ -3520,16 +3675,18 @@
     </row>
     <row r="66" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C66" s="23"/>
       <c r="D66" s="12">
         <v>0.5</v>
       </c>
-      <c r="E66" s="29"/>
+      <c r="E66" s="29">
+        <v>29</v>
+      </c>
       <c r="F66" s="29"/>
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
@@ -3542,16 +3699,18 @@
     </row>
     <row r="67" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C67" s="23"/>
       <c r="D67" s="12">
         <v>0.5</v>
       </c>
-      <c r="E67" s="29"/>
+      <c r="E67" s="29">
+        <v>38</v>
+      </c>
       <c r="F67" s="29"/>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
@@ -3564,16 +3723,18 @@
     </row>
     <row r="68" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C68" s="23"/>
       <c r="D68" s="12">
         <v>0.5</v>
       </c>
-      <c r="E68" s="29"/>
+      <c r="E68" s="29">
+        <v>47</v>
+      </c>
       <c r="F68" s="29"/>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
@@ -3588,16 +3749,18 @@
     </row>
     <row r="69" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C69" s="23"/>
       <c r="D69" s="12">
         <v>0.5</v>
       </c>
-      <c r="E69" s="29"/>
+      <c r="E69" s="29">
+        <v>56</v>
+      </c>
       <c r="F69" s="29"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
@@ -3612,16 +3775,18 @@
     </row>
     <row r="70" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C70" s="23"/>
       <c r="D70" s="12">
         <v>0.5</v>
       </c>
-      <c r="E70" s="29"/>
+      <c r="E70" s="29">
+        <v>65</v>
+      </c>
       <c r="F70" s="29"/>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
@@ -3636,16 +3801,18 @@
     </row>
     <row r="71" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C71" s="23"/>
       <c r="D71" s="12">
         <v>0.5</v>
       </c>
-      <c r="E71" s="29"/>
+      <c r="E71" s="29">
+        <v>74</v>
+      </c>
       <c r="F71" s="29"/>
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
@@ -3660,16 +3827,18 @@
     </row>
     <row r="72" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C72" s="23"/>
       <c r="D72" s="12">
         <v>0.5</v>
       </c>
-      <c r="E72" s="29"/>
+      <c r="E72" s="29">
+        <v>83</v>
+      </c>
       <c r="F72" s="29"/>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
@@ -3684,16 +3853,18 @@
     </row>
     <row r="73" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C73" s="23"/>
       <c r="D73" s="12">
         <v>0.5</v>
       </c>
-      <c r="E73" s="29"/>
+      <c r="E73" s="29">
+        <v>92</v>
+      </c>
       <c r="F73" s="29"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
@@ -3708,16 +3879,18 @@
     </row>
     <row r="74" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C74" s="23"/>
       <c r="D74" s="12">
         <v>0.5</v>
       </c>
-      <c r="E74" s="29"/>
+      <c r="E74" s="29">
+        <v>30</v>
+      </c>
       <c r="F74" s="29"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
@@ -3732,16 +3905,18 @@
     </row>
     <row r="75" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C75" s="23"/>
       <c r="D75" s="12">
         <v>0.5</v>
       </c>
-      <c r="E75" s="29"/>
+      <c r="E75" s="29">
+        <v>39</v>
+      </c>
       <c r="F75" s="29"/>
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
@@ -3756,16 +3931,18 @@
     </row>
     <row r="76" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C76" s="23"/>
       <c r="D76" s="12">
         <v>0.5</v>
       </c>
-      <c r="E76" s="29"/>
+      <c r="E76" s="29">
+        <v>48</v>
+      </c>
       <c r="F76" s="29"/>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
@@ -3780,16 +3957,18 @@
     </row>
     <row r="77" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C77" s="23"/>
       <c r="D77" s="12">
         <v>0.5</v>
       </c>
-      <c r="E77" s="29"/>
+      <c r="E77" s="29">
+        <v>57</v>
+      </c>
       <c r="F77" s="29"/>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
@@ -3804,16 +3983,18 @@
     </row>
     <row r="78" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C78" s="23"/>
       <c r="D78" s="12">
         <v>0.5</v>
       </c>
-      <c r="E78" s="29"/>
+      <c r="E78" s="29">
+        <v>66</v>
+      </c>
       <c r="F78" s="29"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
@@ -3828,16 +4009,18 @@
     </row>
     <row r="79" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C79" s="23"/>
       <c r="D79" s="12">
         <v>0.5</v>
       </c>
-      <c r="E79" s="29"/>
+      <c r="E79" s="29">
+        <v>75</v>
+      </c>
       <c r="F79" s="29"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
@@ -3852,16 +4035,18 @@
     </row>
     <row r="80" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C80" s="23"/>
       <c r="D80" s="12">
         <v>0.5</v>
       </c>
-      <c r="E80" s="29"/>
+      <c r="E80" s="29">
+        <v>84</v>
+      </c>
       <c r="F80" s="29"/>
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
@@ -3876,16 +4061,18 @@
     </row>
     <row r="81" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="12">
         <v>0.5</v>
       </c>
-      <c r="E81" s="29"/>
+      <c r="E81" s="29">
+        <v>93</v>
+      </c>
       <c r="F81" s="29"/>
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
@@ -3900,16 +4087,18 @@
     </row>
     <row r="82" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C82" s="23"/>
       <c r="D82" s="12">
         <v>0.5</v>
       </c>
-      <c r="E82" s="29"/>
+      <c r="E82" s="29">
+        <v>40</v>
+      </c>
       <c r="F82" s="29"/>
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
@@ -3924,16 +4113,18 @@
     </row>
     <row r="83" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C83" s="23"/>
       <c r="D83" s="12">
         <v>0.5</v>
       </c>
-      <c r="E83" s="29"/>
+      <c r="E83" s="29">
+        <v>49</v>
+      </c>
       <c r="F83" s="29"/>
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
@@ -3948,16 +4139,18 @@
     </row>
     <row r="84" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C84" s="23"/>
       <c r="D84" s="12">
         <v>0.5</v>
       </c>
-      <c r="E84" s="29"/>
+      <c r="E84" s="29">
+        <v>58</v>
+      </c>
       <c r="F84" s="29"/>
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
@@ -3973,16 +4166,18 @@
     </row>
     <row r="85" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C85" s="23"/>
       <c r="D85" s="12">
         <v>0.5</v>
       </c>
-      <c r="E85" s="29"/>
+      <c r="E85" s="29">
+        <v>67</v>
+      </c>
       <c r="F85" s="29"/>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
@@ -3998,16 +4193,18 @@
     </row>
     <row r="86" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C86" s="23"/>
       <c r="D86" s="12">
         <v>0.5</v>
       </c>
-      <c r="E86" s="29"/>
+      <c r="E86" s="29">
+        <v>76</v>
+      </c>
       <c r="F86" s="29"/>
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
@@ -4023,16 +4220,18 @@
     </row>
     <row r="87" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B87" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C87" s="23"/>
       <c r="D87" s="12">
         <v>0.5</v>
       </c>
-      <c r="E87" s="29"/>
+      <c r="E87" s="29">
+        <v>85</v>
+      </c>
       <c r="F87" s="29"/>
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
@@ -4048,16 +4247,18 @@
     </row>
     <row r="88" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B88" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C88" s="23"/>
       <c r="D88" s="12">
         <v>0.5</v>
       </c>
-      <c r="E88" s="29"/>
+      <c r="E88" s="29">
+        <v>94</v>
+      </c>
       <c r="F88" s="29"/>
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
@@ -4073,16 +4274,18 @@
     </row>
     <row r="89" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B89" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C89" s="23"/>
       <c r="D89" s="12">
         <v>0.5</v>
       </c>
-      <c r="E89" s="29"/>
+      <c r="E89" s="29">
+        <v>50</v>
+      </c>
       <c r="F89" s="29"/>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
@@ -4098,16 +4301,18 @@
     </row>
     <row r="90" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B90" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C90" s="23"/>
       <c r="D90" s="12">
         <v>0.5</v>
       </c>
-      <c r="E90" s="29"/>
+      <c r="E90" s="29">
+        <v>59</v>
+      </c>
       <c r="F90" s="29"/>
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
@@ -4122,16 +4327,18 @@
     </row>
     <row r="91" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B91" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C91" s="23"/>
       <c r="D91" s="12">
         <v>0.5</v>
       </c>
-      <c r="E91" s="29"/>
+      <c r="E91" s="29">
+        <v>68</v>
+      </c>
       <c r="F91" s="29"/>
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
@@ -4146,16 +4353,18 @@
     </row>
     <row r="92" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B92" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C92" s="23"/>
       <c r="D92" s="12">
         <v>0.5</v>
       </c>
-      <c r="E92" s="29"/>
+      <c r="E92" s="29">
+        <v>77</v>
+      </c>
       <c r="F92" s="29"/>
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
@@ -4170,16 +4379,18 @@
     </row>
     <row r="93" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B93" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C93" s="23"/>
       <c r="D93" s="12">
         <v>0.5</v>
       </c>
-      <c r="E93" s="29"/>
+      <c r="E93" s="29">
+        <v>86</v>
+      </c>
       <c r="F93" s="29"/>
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
@@ -4194,16 +4405,18 @@
     </row>
     <row r="94" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B94" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C94" s="23"/>
       <c r="D94" s="12">
         <v>0.5</v>
       </c>
-      <c r="E94" s="29"/>
+      <c r="E94" s="29">
+        <v>95</v>
+      </c>
       <c r="F94" s="29"/>
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
@@ -4218,16 +4431,18 @@
     </row>
     <row r="95" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B95" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C95" s="23"/>
       <c r="D95" s="12">
         <v>0.5</v>
       </c>
-      <c r="E95" s="29"/>
+      <c r="E95" s="29">
+        <v>60</v>
+      </c>
       <c r="F95" s="29"/>
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
@@ -4242,16 +4457,18 @@
     </row>
     <row r="96" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C96" s="23"/>
       <c r="D96" s="12">
         <v>0.5</v>
       </c>
-      <c r="E96" s="29"/>
+      <c r="E96" s="29">
+        <v>69</v>
+      </c>
       <c r="F96" s="29"/>
       <c r="G96" s="7"/>
       <c r="H96" s="7"/>
@@ -4266,16 +4483,18 @@
     </row>
     <row r="97" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C97" s="23"/>
       <c r="D97" s="12">
         <v>0.5</v>
       </c>
-      <c r="E97" s="29"/>
+      <c r="E97" s="29">
+        <v>78</v>
+      </c>
       <c r="F97" s="29"/>
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
@@ -4290,16 +4509,18 @@
     </row>
     <row r="98" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B98" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C98" s="23"/>
       <c r="D98" s="12">
         <v>0.5</v>
       </c>
-      <c r="E98" s="29"/>
+      <c r="E98" s="29">
+        <v>87</v>
+      </c>
       <c r="F98" s="29"/>
       <c r="G98" s="7"/>
       <c r="H98" s="7"/>
@@ -4314,16 +4535,18 @@
     </row>
     <row r="99" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B99" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C99" s="23"/>
       <c r="D99" s="12">
         <v>0.5</v>
       </c>
-      <c r="E99" s="29"/>
+      <c r="E99" s="29">
+        <v>96</v>
+      </c>
       <c r="F99" s="29"/>
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
@@ -4338,16 +4561,18 @@
     </row>
     <row r="100" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B100" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C100" s="23"/>
       <c r="D100" s="12">
         <v>0.5</v>
       </c>
-      <c r="E100" s="29"/>
+      <c r="E100" s="29">
+        <v>70</v>
+      </c>
       <c r="F100" s="29"/>
       <c r="G100" s="7"/>
       <c r="H100" s="7"/>
@@ -4362,16 +4587,18 @@
     </row>
     <row r="101" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C101" s="23"/>
       <c r="D101" s="12">
         <v>0.5</v>
       </c>
-      <c r="E101" s="29"/>
+      <c r="E101" s="29">
+        <v>79</v>
+      </c>
       <c r="F101" s="29"/>
       <c r="G101" s="7"/>
       <c r="H101" s="7"/>
@@ -4386,16 +4613,18 @@
     </row>
     <row r="102" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B102" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C102" s="23"/>
       <c r="D102" s="12">
         <v>0.5</v>
       </c>
-      <c r="E102" s="29"/>
+      <c r="E102" s="29">
+        <v>88</v>
+      </c>
       <c r="F102" s="29"/>
       <c r="G102" s="7"/>
       <c r="H102" s="7"/>
@@ -4410,16 +4639,18 @@
     </row>
     <row r="103" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B103" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C103" s="23"/>
       <c r="D103" s="12">
         <v>0.5</v>
       </c>
-      <c r="E103" s="29"/>
+      <c r="E103" s="29">
+        <v>97</v>
+      </c>
       <c r="F103" s="29"/>
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
@@ -4452,17 +4683,21 @@
     </row>
     <row r="105" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C105" s="23"/>
       <c r="D105" s="12">
         <v>1</v>
       </c>
-      <c r="E105" s="29"/>
-      <c r="F105" s="29"/>
+      <c r="E105" s="29">
+        <v>13</v>
+      </c>
+      <c r="F105" s="29" t="s">
+        <v>167</v>
+      </c>
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
@@ -4476,16 +4711,18 @@
     </row>
     <row r="106" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B106" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C106" s="23"/>
       <c r="D106" s="12">
         <v>1</v>
       </c>
-      <c r="E106" s="29"/>
+      <c r="E106" s="29">
+        <v>14</v>
+      </c>
       <c r="F106" s="29"/>
       <c r="G106" s="7"/>
       <c r="H106" s="7"/>
@@ -4500,16 +4737,18 @@
     </row>
     <row r="107" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C107" s="23"/>
       <c r="D107" s="12">
         <v>1</v>
       </c>
-      <c r="E107" s="29"/>
+      <c r="E107" s="29">
+        <v>15</v>
+      </c>
       <c r="F107" s="29"/>
       <c r="G107" s="7"/>
       <c r="H107" s="7"/>
@@ -4524,16 +4763,18 @@
     </row>
     <row r="108" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B108" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C108" s="23"/>
       <c r="D108" s="12">
         <v>1</v>
       </c>
-      <c r="E108" s="29"/>
+      <c r="E108" s="29">
+        <v>16</v>
+      </c>
       <c r="F108" s="29"/>
       <c r="G108" s="7"/>
       <c r="H108" s="7"/>
@@ -4548,16 +4789,18 @@
     </row>
     <row r="109" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B109" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C109" s="23"/>
       <c r="D109" s="12">
         <v>1</v>
       </c>
-      <c r="E109" s="29"/>
+      <c r="E109" s="29">
+        <v>17</v>
+      </c>
       <c r="F109" s="29"/>
       <c r="G109" s="7"/>
       <c r="H109" s="7"/>
@@ -4572,16 +4815,18 @@
     </row>
     <row r="110" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B110" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C110" s="23"/>
       <c r="D110" s="12">
         <v>1</v>
       </c>
-      <c r="E110" s="29"/>
+      <c r="E110" s="29">
+        <v>18</v>
+      </c>
       <c r="F110" s="29"/>
       <c r="G110" s="7"/>
       <c r="H110" s="7"/>
@@ -4596,16 +4841,18 @@
     </row>
     <row r="111" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B111" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C111" s="23"/>
       <c r="D111" s="12">
         <v>1</v>
       </c>
-      <c r="E111" s="29"/>
+      <c r="E111" s="29">
+        <v>19</v>
+      </c>
       <c r="F111" s="29"/>
       <c r="G111" s="7"/>
       <c r="H111" s="7"/>
@@ -4620,16 +4867,18 @@
     </row>
     <row r="112" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B112" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C112" s="23"/>
       <c r="D112" s="12">
         <v>1</v>
       </c>
-      <c r="E112" s="29"/>
+      <c r="E112" s="29">
+        <v>20</v>
+      </c>
       <c r="F112" s="29"/>
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>
@@ -4644,16 +4893,18 @@
     </row>
     <row r="113" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B113" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C113" s="23"/>
       <c r="D113" s="12">
         <v>1</v>
       </c>
-      <c r="E113" s="29"/>
+      <c r="E113" s="29">
+        <v>21</v>
+      </c>
       <c r="F113" s="29"/>
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
@@ -4668,16 +4919,18 @@
     </row>
     <row r="114" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B114" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C114" s="23"/>
       <c r="D114" s="12">
         <v>1</v>
       </c>
-      <c r="E114" s="29"/>
+      <c r="E114" s="29">
+        <v>22</v>
+      </c>
       <c r="F114" s="29"/>
       <c r="G114" s="7"/>
       <c r="H114" s="7"/>
@@ -4692,16 +4945,18 @@
     </row>
     <row r="115" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B115" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C115" s="23"/>
       <c r="D115" s="12">
         <v>1</v>
       </c>
-      <c r="E115" s="29"/>
+      <c r="E115" s="29">
+        <v>23</v>
+      </c>
       <c r="F115" s="29"/>
       <c r="G115" s="7"/>
       <c r="H115" s="7"/>
@@ -4716,16 +4971,18 @@
     </row>
     <row r="116" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B116" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C116" s="23"/>
       <c r="D116" s="12">
         <v>1</v>
       </c>
-      <c r="E116" s="29"/>
+      <c r="E116" s="29">
+        <v>24</v>
+      </c>
       <c r="F116" s="29"/>
       <c r="G116" s="7"/>
       <c r="H116" s="7"/>
@@ -4740,16 +4997,18 @@
     </row>
     <row r="117" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B117" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C117" s="23"/>
       <c r="D117" s="12">
         <v>1</v>
       </c>
-      <c r="E117" s="29"/>
+      <c r="E117" s="29">
+        <v>33</v>
+      </c>
       <c r="F117" s="29"/>
       <c r="G117" s="7"/>
       <c r="H117" s="7"/>
@@ -4764,16 +5023,18 @@
     </row>
     <row r="118" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B118" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C118" s="23"/>
       <c r="D118" s="12">
         <v>1</v>
       </c>
-      <c r="E118" s="29"/>
+      <c r="E118" s="29">
+        <v>34</v>
+      </c>
       <c r="F118" s="29"/>
       <c r="G118" s="7"/>
       <c r="H118" s="7"/>
@@ -4788,16 +5049,18 @@
     </row>
     <row r="119" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B119" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C119" s="23"/>
       <c r="D119" s="12">
         <v>1</v>
       </c>
-      <c r="E119" s="29"/>
+      <c r="E119" s="29">
+        <v>35</v>
+      </c>
       <c r="F119" s="29"/>
       <c r="G119" s="7"/>
       <c r="H119" s="7"/>
@@ -4812,16 +5075,18 @@
     </row>
     <row r="120" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B120" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C120" s="23"/>
       <c r="D120" s="12">
         <v>1</v>
       </c>
-      <c r="E120" s="29"/>
+      <c r="E120" s="29">
+        <v>36</v>
+      </c>
       <c r="F120" s="29"/>
       <c r="G120" s="7"/>
       <c r="H120" s="7"/>
@@ -4854,7 +5119,7 @@
     </row>
     <row r="122" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -4874,17 +5139,21 @@
     </row>
     <row r="123" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C123" s="23"/>
       <c r="D123" s="12">
         <v>2</v>
       </c>
-      <c r="E123" s="29"/>
-      <c r="F123" s="29"/>
+      <c r="E123" s="29">
+        <v>11</v>
+      </c>
+      <c r="F123" s="29" t="s">
+        <v>168</v>
+      </c>
       <c r="G123" s="7"/>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
@@ -4898,16 +5167,18 @@
     </row>
     <row r="124" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C124" s="23"/>
       <c r="D124" s="12">
         <v>2</v>
       </c>
-      <c r="E124" s="29"/>
+      <c r="E124" s="29">
+        <v>21</v>
+      </c>
       <c r="F124" s="29"/>
       <c r="G124" s="7"/>
       <c r="H124" s="7"/>
@@ -4922,16 +5193,18 @@
     </row>
     <row r="125" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C125" s="23"/>
       <c r="D125" s="12">
         <v>2</v>
       </c>
-      <c r="E125" s="29"/>
+      <c r="E125" s="29">
+        <v>22</v>
+      </c>
       <c r="F125" s="29"/>
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
@@ -4946,16 +5219,18 @@
     </row>
     <row r="126" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C126" s="23"/>
       <c r="D126" s="12">
         <v>1</v>
       </c>
-      <c r="E126" s="29"/>
+      <c r="E126" s="29">
+        <v>23</v>
+      </c>
       <c r="F126" s="29"/>
       <c r="G126" s="7"/>
       <c r="H126" s="7"/>
@@ -4970,16 +5245,18 @@
     </row>
     <row r="127" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C127" s="23"/>
       <c r="D127" s="12">
         <v>1</v>
       </c>
-      <c r="E127" s="29"/>
+      <c r="E127" s="29">
+        <v>24</v>
+      </c>
       <c r="F127" s="29"/>
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
@@ -4994,16 +5271,18 @@
     </row>
     <row r="128" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B128" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C128" s="23"/>
       <c r="D128" s="12">
         <v>1</v>
       </c>
-      <c r="E128" s="29"/>
+      <c r="E128" s="29">
+        <v>25</v>
+      </c>
       <c r="F128" s="29"/>
       <c r="G128" s="7"/>
       <c r="H128" s="7"/>
@@ -5018,10 +5297,10 @@
     </row>
     <row r="129" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B129" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C129" s="7"/>
       <c r="D129" s="12"/>
@@ -5040,16 +5319,18 @@
     </row>
     <row r="130" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B130" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C130" s="23"/>
       <c r="D130" s="12">
         <v>1</v>
       </c>
-      <c r="E130" s="29"/>
+      <c r="E130" s="29">
+        <v>26</v>
+      </c>
       <c r="F130" s="29"/>
       <c r="G130" s="7"/>
       <c r="H130" s="7"/>
@@ -5064,16 +5345,18 @@
     </row>
     <row r="131" spans="1:256" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C131" s="23"/>
       <c r="D131" s="12">
         <v>1</v>
       </c>
-      <c r="E131" s="29"/>
+      <c r="E131" s="29">
+        <v>27</v>
+      </c>
       <c r="F131" s="29"/>
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>
@@ -5088,10 +5371,10 @@
     </row>
     <row r="132" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B132" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C132" s="20"/>
       <c r="D132" s="27"/>
@@ -5107,16 +5390,18 @@
     </row>
     <row r="133" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B133" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C133" s="21"/>
       <c r="D133" s="12">
         <v>1</v>
       </c>
-      <c r="E133" s="22"/>
+      <c r="E133" s="22">
+        <v>28</v>
+      </c>
       <c r="F133" s="22"/>
       <c r="G133" s="20"/>
       <c r="H133" s="20"/>
@@ -5128,16 +5413,18 @@
     </row>
     <row r="134" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B134" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C134" s="21"/>
       <c r="D134" s="12">
         <v>1</v>
       </c>
-      <c r="E134" s="22"/>
+      <c r="E134" s="22">
+        <v>29</v>
+      </c>
       <c r="F134" s="22"/>
       <c r="G134" s="20"/>
       <c r="H134" s="20"/>
@@ -5149,16 +5436,18 @@
     </row>
     <row r="135" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B135" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C135" s="21"/>
       <c r="D135" s="12">
         <v>1</v>
       </c>
-      <c r="E135" s="22"/>
+      <c r="E135" s="22">
+        <v>30</v>
+      </c>
       <c r="F135" s="22"/>
       <c r="G135" s="20"/>
       <c r="H135" s="20"/>
@@ -5170,10 +5459,10 @@
     </row>
     <row r="136" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B136" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C136" s="20"/>
       <c r="D136" s="27"/>
@@ -5189,16 +5478,18 @@
     </row>
     <row r="137" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C137" s="21"/>
       <c r="D137" s="12">
         <v>1</v>
       </c>
-      <c r="E137" s="22"/>
+      <c r="E137" s="22">
+        <v>31</v>
+      </c>
       <c r="F137" s="22"/>
       <c r="G137" s="20"/>
       <c r="H137" s="20"/>
@@ -5210,10 +5501,10 @@
     </row>
     <row r="138" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C138" s="20"/>
       <c r="D138" s="27"/>
@@ -5229,16 +5520,18 @@
     </row>
     <row r="139" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C139" s="21"/>
       <c r="D139" s="12">
         <v>1</v>
       </c>
-      <c r="E139" s="22"/>
+      <c r="E139" s="22">
+        <v>32</v>
+      </c>
       <c r="F139" s="22"/>
       <c r="G139" s="20"/>
       <c r="H139" s="20"/>
@@ -5250,10 +5543,10 @@
     </row>
     <row r="140" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B140" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C140" s="20"/>
       <c r="D140" s="27"/>
@@ -5269,16 +5562,18 @@
     </row>
     <row r="141" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C141" s="21"/>
       <c r="D141" s="12">
         <v>1</v>
       </c>
-      <c r="E141" s="22"/>
+      <c r="E141" s="22">
+        <v>33</v>
+      </c>
       <c r="F141" s="22"/>
       <c r="G141" s="20"/>
       <c r="H141" s="20"/>
@@ -5290,16 +5585,18 @@
     </row>
     <row r="142" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B142" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C142" s="21"/>
       <c r="D142" s="12">
         <v>1</v>
       </c>
-      <c r="E142" s="22"/>
+      <c r="E142" s="22">
+        <v>43</v>
+      </c>
       <c r="F142" s="22"/>
       <c r="G142" s="20"/>
       <c r="H142" s="20"/>
@@ -5311,16 +5608,18 @@
     </row>
     <row r="143" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B143" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C143" s="21"/>
       <c r="D143" s="12">
         <v>1</v>
       </c>
-      <c r="E143" s="22"/>
+      <c r="E143" s="22">
+        <v>44</v>
+      </c>
       <c r="F143" s="22"/>
       <c r="G143" s="20"/>
       <c r="H143" s="20"/>
@@ -5332,10 +5631,10 @@
     </row>
     <row r="144" spans="1:256" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B144" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C144" s="20"/>
       <c r="D144" s="27"/>
@@ -5351,16 +5650,18 @@
     </row>
     <row r="145" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B145" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C145" s="21"/>
       <c r="D145" s="12">
         <v>1</v>
       </c>
-      <c r="E145" s="22"/>
+      <c r="E145" s="22">
+        <v>45</v>
+      </c>
       <c r="F145" s="22"/>
       <c r="G145" s="20"/>
       <c r="H145" s="20"/>
@@ -5372,10 +5673,10 @@
     </row>
     <row r="146" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B146" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C146" s="20"/>
       <c r="D146" s="27"/>
@@ -5391,16 +5692,18 @@
     </row>
     <row r="147" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C147" s="21"/>
       <c r="D147" s="12">
         <v>1</v>
       </c>
-      <c r="E147" s="22"/>
+      <c r="E147" s="22">
+        <v>46</v>
+      </c>
       <c r="F147" s="22"/>
       <c r="G147" s="20"/>
       <c r="H147" s="20"/>
@@ -5412,10 +5715,10 @@
     </row>
     <row r="148" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B148" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C148" s="20"/>
       <c r="D148" s="27"/>
@@ -5431,16 +5734,18 @@
     </row>
     <row r="149" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149" s="22" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C149" s="21"/>
       <c r="D149" s="12">
         <v>1</v>
       </c>
-      <c r="E149" s="22"/>
+      <c r="E149" s="22">
+        <v>47</v>
+      </c>
       <c r="F149" s="22"/>
       <c r="G149" s="20"/>
       <c r="H149" s="20"/>
@@ -5467,7 +5772,7 @@
     </row>
     <row r="151" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B151" s="20"/>
       <c r="C151" s="20"/>

</xml_diff>